<commit_message>
Team Rankings initialised on Database
Now reading through CSV and implemented through code first entity
framework.
</commit_message>
<xml_diff>
--- a/Blob storage/TeamRanking.xlsx
+++ b/Blob storage/TeamRanking.xlsx
@@ -1707,13 +1707,13 @@
     <t>TeamName</t>
   </si>
   <si>
-    <t>Position</t>
-  </si>
-  <si>
     <t>Ranking</t>
   </si>
   <si>
     <t>CountryCode</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -2057,7 +2057,7 @@
   <dimension ref="A1:F509"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,16 +2070,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="B1" t="s">
         <v>562</v>
       </c>
       <c r="C1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>

</xml_diff>